<commit_message>
Update module 3 template
</commit_message>
<xml_diff>
--- a/public/templates/NHWA_Module_3.xlsx
+++ b/public/templates/NHWA_Module_3.xlsx
@@ -5,18 +5,18 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\NHWA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\NHWA\Originals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7364344-FFBC-4503-A1F3-68601D9D6B60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DNdhLaiJYJ2ZbD09elSFCyIbsfmsCvuMR7TLpKKqcWr+WHl4whasq0ZZ0A0eyWjFnXr15kGsuJqYxaWBtC5Tlw==" workbookSaltValue="6xngd8mX30SibXiPrW6QDg==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A467AA-1D46-4723-912D-E8ED25B57169}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hSTKI/Kp4ZNeltw23FK/qSJ4IP1EgotV+JfeQVdh4yL1WlROhPptf/kQIRKuiu2N/Uq0Rm59grAA/Oi+aswdHA==" workbookSaltValue="XnyCBAHZzk/HLZuhAG6zhw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11775" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regulation" sheetId="1" r:id="rId1"/>
     <sheet name="Acreditation" sheetId="5" r:id="rId2"/>
-    <sheet name="Lifelong Learning " sheetId="6" r:id="rId3"/>
+    <sheet name="Lifelong Learning" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -2863,12 +2863,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -9242,22 +9242,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="49" t="s">
         <v>840</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>758</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
@@ -9287,18 +9287,18 @@
       </c>
     </row>
     <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="33"/>
       <c r="L2" s="33"/>
       <c r="M2" s="33"/>
@@ -17855,42 +17855,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>758</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:46" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
       <c r="AT2" s="25" t="e">
         <f>Regulation!X2</f>
         <v>#N/A</v>
@@ -20731,42 +20731,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="50" t="s">
         <v>758</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
     </row>
     <row r="2" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="50" t="s">
         <v>743</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
       <c r="W2" s="25" t="e">
         <f>Regulation!X2</f>
         <v>#N/A</v>

</xml_diff>